<commit_message>
language update: detailed adjustments uuid
</commit_message>
<xml_diff>
--- a/src/UPDATE/base_data/UPDATE_glacier_description_FR.xlsx
+++ b/src/UPDATE/base_data/UPDATE_glacier_description_FR.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="9465" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="9465"/>
   </bookViews>
   <sheets>
     <sheet name="fr" sheetId="8" r:id="rId1"/>
@@ -1442,9 +1442,6 @@
     <t>801e8670-4ec8-11e8-9ca9-985fd331b2ee</t>
   </si>
   <si>
-    <t>81722f8f-4ec8-11e8-8842-985fd331b2ee</t>
-  </si>
-  <si>
     <t>80f425f0-4ec8-11e8-81a5-985fd331b2ee</t>
   </si>
   <si>
@@ -1493,9 +1490,6 @@
     <t>Geltengletscher</t>
   </si>
   <si>
-    <t>810ae240-4ec8-11e8-9773-985fd331b2ee</t>
-  </si>
-  <si>
     <t>810d051e-4ec8-11e8-8e0f-985fd331b2ee</t>
   </si>
   <si>
@@ -1853,9 +1847,6 @@
     <t>82098d8f-4ec8-11e8-936e-985fd331b2ee</t>
   </si>
   <si>
-    <t>81e98270-4ec8-11e8-86b3-985fd331b2ee</t>
-  </si>
-  <si>
     <t>81ec1a80-4ec8-11e8-8d89-985fd331b2ee</t>
   </si>
   <si>
@@ -2514,6 +2505,15 @@
   </si>
   <si>
     <t>UPDATE base_data.glacier_description SET description = 'Le glacier de Zmutt se trouve dans le canton du Valais. Il a une superficie de 13.74 km2 et sa longueur est de 7.87 km (données de 2010). En 1973, le glacier avait une superficie de 16.85 km2. Le changement de superficie relatif équivaut à -18.48 %. Le glacier se termine en une langue plate et hautement couverte de débris.' WHERE fk_glacier='7f9a3b40-4ec8-11e8-9c5e-985fd331b2ee' AND fk_language_type='fr' AND fk_glacier_description_type ='0';</t>
+  </si>
+  <si>
+    <t>8176754f-4ec8-11e8-9a29-985fd331b2ee</t>
+  </si>
+  <si>
+    <t>81103970-4ec8-11e8-8d3b-985fd331b2ee</t>
+  </si>
+  <si>
+    <t>81ed04e1-4ec8-11e8-a1f7-985fd331b2ee</t>
   </si>
 </sst>
 </file>
@@ -2908,17 +2908,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G162"/>
   <sheetViews>
-    <sheetView topLeftCell="B132" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B147" sqref="A147:XFD147"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A147" sqref="A147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
     <col min="3" max="3" width="33.28515625" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="2.5703125" customWidth="1"/>
     <col min="6" max="6" width="76.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2927,7 +2927,7 @@
         <v>454</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C1" t="s">
         <v>450</v>
@@ -2942,7 +2942,7 @@
         <v>453</v>
       </c>
       <c r="G1" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2965,7 +2965,7 @@
         <v>297</v>
       </c>
       <c r="G2" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3011,7 +3011,7 @@
         <v>339</v>
       </c>
       <c r="G4" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3034,7 +3034,7 @@
         <v>393</v>
       </c>
       <c r="G5" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3126,7 +3126,7 @@
         <v>342</v>
       </c>
       <c r="G9" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3218,7 +3218,7 @@
         <v>336</v>
       </c>
       <c r="G13" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3241,7 +3241,7 @@
         <v>421</v>
       </c>
       <c r="G14" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3269,7 +3269,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>470</v>
+        <v>825</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>31</v>
@@ -3284,15 +3284,15 @@
         <v>144</v>
       </c>
       <c r="F16" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="G16" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>20</v>
@@ -3310,12 +3310,12 @@
         <v>321</v>
       </c>
       <c r="G17" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>34</v>
@@ -3338,7 +3338,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>43</v>
@@ -3356,12 +3356,12 @@
         <v>368</v>
       </c>
       <c r="G19" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>5</v>
@@ -3379,12 +3379,12 @@
         <v>289</v>
       </c>
       <c r="G20" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>37</v>
@@ -3407,7 +3407,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>1</v>
@@ -3430,10 +3430,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>477</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>478</v>
       </c>
       <c r="C23" t="s">
         <v>442</v>
@@ -3445,15 +3445,15 @@
         <v>144</v>
       </c>
       <c r="F23" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="G23" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>106</v>
@@ -3471,12 +3471,12 @@
         <v>392</v>
       </c>
       <c r="G24" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>127</v>
@@ -3494,12 +3494,12 @@
         <v>334</v>
       </c>
       <c r="G25" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>23</v>
@@ -3522,7 +3522,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>38</v>
@@ -3545,10 +3545,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>485</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>486</v>
       </c>
       <c r="C28" t="s">
         <v>445</v>
@@ -3568,7 +3568,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>46</v>
@@ -3591,7 +3591,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>7</v>
@@ -3614,7 +3614,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>487</v>
+        <v>826</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>88</v>
@@ -3629,15 +3629,15 @@
         <v>144</v>
       </c>
       <c r="F31" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="G31" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>139</v>
@@ -3660,7 +3660,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>117</v>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>110</v>
@@ -3706,7 +3706,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>116</v>
@@ -3729,7 +3729,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>131</v>
@@ -3752,7 +3752,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>125</v>
@@ -3775,7 +3775,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>57</v>
@@ -3798,7 +3798,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B39" s="13" t="s">
         <v>64</v>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B40" s="14" t="s">
         <v>86</v>
@@ -3839,15 +3839,15 @@
         <v>350</v>
       </c>
       <c r="G40" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C41" t="s">
         <v>440</v>
@@ -3859,15 +3859,15 @@
         <v>144</v>
       </c>
       <c r="F41" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="G41" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>91</v>
@@ -3890,7 +3890,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B43" s="14" t="s">
         <v>96</v>
@@ -3908,12 +3908,12 @@
         <v>374</v>
       </c>
       <c r="G43" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>75</v>
@@ -3936,7 +3936,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>72</v>
@@ -3959,7 +3959,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>141</v>
@@ -3982,7 +3982,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>111</v>
@@ -4005,7 +4005,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>66</v>
@@ -4028,7 +4028,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>104</v>
@@ -4051,7 +4051,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>95</v>
@@ -4074,7 +4074,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>126</v>
@@ -4097,7 +4097,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>87</v>
@@ -4120,10 +4120,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C53" t="s">
         <v>439</v>
@@ -4143,7 +4143,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>59</v>
@@ -4166,7 +4166,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>109</v>
@@ -4189,7 +4189,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>97</v>
@@ -4207,12 +4207,12 @@
         <v>375</v>
       </c>
       <c r="G56" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B57" s="15" t="s">
         <v>61</v>
@@ -4230,12 +4230,12 @@
         <v>293</v>
       </c>
       <c r="G57" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>123</v>
@@ -4258,7 +4258,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>73</v>
@@ -4273,15 +4273,15 @@
         <v>144</v>
       </c>
       <c r="F59" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="G59" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>135</v>
@@ -4304,7 +4304,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>70</v>
@@ -4327,7 +4327,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>68</v>
@@ -4350,7 +4350,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>62</v>
@@ -4373,7 +4373,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>114</v>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>112</v>
@@ -4419,7 +4419,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>69</v>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>94</v>
@@ -4465,7 +4465,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>133</v>
@@ -4488,7 +4488,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>101</v>
@@ -4511,7 +4511,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>90</v>
@@ -4534,7 +4534,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>103</v>
@@ -4557,7 +4557,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>99</v>
@@ -4580,7 +4580,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>78</v>
@@ -4598,12 +4598,12 @@
         <v>330</v>
       </c>
       <c r="G73" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>0</v>
@@ -4626,7 +4626,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>17</v>
@@ -4641,15 +4641,15 @@
         <v>144</v>
       </c>
       <c r="F75" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G75" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>48</v>
@@ -4667,12 +4667,12 @@
         <v>383</v>
       </c>
       <c r="G76" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B77" s="16" t="s">
         <v>48</v>
@@ -4690,12 +4690,12 @@
         <v>398</v>
       </c>
       <c r="G77" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>56</v>
@@ -4710,15 +4710,15 @@
         <v>144</v>
       </c>
       <c r="F78" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="G78" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>39</v>
@@ -4741,7 +4741,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B80" s="14" t="s">
         <v>77</v>
@@ -4759,12 +4759,12 @@
         <v>327</v>
       </c>
       <c r="G80" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>41</v>
@@ -4787,7 +4787,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B82" s="16" t="s">
         <v>446</v>
@@ -4810,7 +4810,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>42</v>
@@ -4833,10 +4833,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C84" t="s">
         <v>24</v>
@@ -4856,7 +4856,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>33</v>
@@ -4879,7 +4879,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>19</v>
@@ -4902,7 +4902,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>120</v>
@@ -4925,7 +4925,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>60</v>
@@ -4943,12 +4943,12 @@
         <v>292</v>
       </c>
       <c r="G88" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>44</v>
@@ -4971,7 +4971,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>105</v>
@@ -4994,7 +4994,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>9</v>
@@ -5009,15 +5009,15 @@
         <v>144</v>
       </c>
       <c r="F91" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="G91" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>100</v>
@@ -5040,7 +5040,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>129</v>
@@ -5063,7 +5063,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>18</v>
@@ -5086,7 +5086,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>30</v>
@@ -5109,7 +5109,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B96" s="8" t="s">
         <v>12</v>
@@ -5127,12 +5127,12 @@
         <v>303</v>
       </c>
       <c r="G96" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>52</v>
@@ -5155,7 +5155,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>21</v>
@@ -5173,12 +5173,12 @@
         <v>322</v>
       </c>
       <c r="G98" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>3</v>
@@ -5196,15 +5196,15 @@
         <v>285</v>
       </c>
       <c r="G99" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C100" t="s">
         <v>63</v>
@@ -5224,7 +5224,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>79</v>
@@ -5247,7 +5247,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>55</v>
@@ -5265,12 +5265,12 @@
         <v>416</v>
       </c>
       <c r="G102" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>35</v>
@@ -5293,7 +5293,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>54</v>
@@ -5311,15 +5311,15 @@
         <v>437</v>
       </c>
       <c r="G104" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C105" t="s">
         <v>115</v>
@@ -5339,7 +5339,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B106" s="8" t="s">
         <v>140</v>
@@ -5362,7 +5362,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B107" s="8" t="s">
         <v>4</v>
@@ -5377,15 +5377,15 @@
         <v>144</v>
       </c>
       <c r="F107" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="G107" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B108" s="8" t="s">
         <v>10</v>
@@ -5408,7 +5408,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B109" s="8" t="s">
         <v>13</v>
@@ -5431,7 +5431,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B110" s="8" t="s">
         <v>134</v>
@@ -5454,7 +5454,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B111" s="10" t="s">
         <v>447</v>
@@ -5472,12 +5472,12 @@
         <v>448</v>
       </c>
       <c r="G111" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B112" s="10" t="s">
         <v>444</v>
@@ -5500,7 +5500,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>142</v>
@@ -5515,15 +5515,15 @@
         <v>144</v>
       </c>
       <c r="F113" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="G113" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B114" s="8" t="s">
         <v>138</v>
@@ -5546,7 +5546,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B115" s="8" t="s">
         <v>53</v>
@@ -5569,7 +5569,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>15</v>
@@ -5592,7 +5592,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B117" s="8" t="s">
         <v>47</v>
@@ -5615,7 +5615,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B118" s="13" t="s">
         <v>132</v>
@@ -5638,7 +5638,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B119" s="8" t="s">
         <v>26</v>
@@ -5653,15 +5653,15 @@
         <v>144</v>
       </c>
       <c r="F119" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="G119" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B120" s="8" t="s">
         <v>11</v>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B121" s="8" t="s">
         <v>49</v>
@@ -5707,7 +5707,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B122" s="10" t="s">
         <v>449</v>
@@ -5730,7 +5730,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="8" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B123" s="8" t="s">
         <v>36</v>
@@ -5748,12 +5748,12 @@
         <v>347</v>
       </c>
       <c r="G123" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="9" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B124" s="9" t="s">
         <v>83</v>
@@ -5776,7 +5776,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="8" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B125" s="8" t="s">
         <v>121</v>
@@ -5799,7 +5799,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B126" s="8" t="s">
         <v>93</v>
@@ -5822,7 +5822,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="9" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B127" s="9" t="s">
         <v>82</v>
@@ -5845,7 +5845,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B128" s="8" t="s">
         <v>14</v>
@@ -5868,7 +5868,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="8" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B129" s="8" t="s">
         <v>136</v>
@@ -5891,7 +5891,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B130" s="8" t="s">
         <v>16</v>
@@ -5914,7 +5914,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B131" s="8" t="s">
         <v>2</v>
@@ -5929,15 +5929,15 @@
         <v>144</v>
       </c>
       <c r="F131" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="G131" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B132" s="8" t="s">
         <v>119</v>
@@ -5955,12 +5955,12 @@
         <v>438</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B133" s="8" t="s">
         <v>76</v>
@@ -5983,7 +5983,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="12" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B134" s="8" t="s">
         <v>84</v>
@@ -6006,7 +6006,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B135" s="14" t="s">
         <v>80</v>
@@ -6024,12 +6024,12 @@
         <v>333</v>
       </c>
       <c r="G135" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B136" s="8" t="s">
         <v>67</v>
@@ -6052,7 +6052,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B137" s="8" t="s">
         <v>107</v>
@@ -6075,7 +6075,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B138" s="8" t="s">
         <v>102</v>
@@ -6098,7 +6098,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B139" s="8" t="s">
         <v>85</v>
@@ -6121,7 +6121,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B140" s="8" t="s">
         <v>58</v>
@@ -6144,7 +6144,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>71</v>
@@ -6167,7 +6167,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B142" s="8" t="s">
         <v>92</v>
@@ -6190,7 +6190,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B143" s="8" t="s">
         <v>65</v>
@@ -6213,7 +6213,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B144" s="8" t="s">
         <v>108</v>
@@ -6236,7 +6236,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="8" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B145" s="8" t="s">
         <v>74</v>
@@ -6259,7 +6259,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B146" s="8" t="s">
         <v>98</v>
@@ -6282,7 +6282,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="8" t="s">
-        <v>607</v>
+        <v>827</v>
       </c>
       <c r="B147" s="8" t="s">
         <v>441</v>
@@ -6297,15 +6297,15 @@
         <v>144</v>
       </c>
       <c r="F147" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="G147" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="B148" s="8" t="s">
         <v>89</v>
@@ -6328,7 +6328,7 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="8" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="B149" s="8" t="s">
         <v>130</v>
@@ -6351,7 +6351,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="8" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="B150" s="8" t="s">
         <v>113</v>
@@ -6374,7 +6374,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>137</v>
@@ -6397,7 +6397,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B152" s="8" t="s">
         <v>45</v>
@@ -6415,12 +6415,12 @@
         <v>373</v>
       </c>
       <c r="G152" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="B153" s="8" t="s">
         <v>40</v>
@@ -6443,7 +6443,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B154" s="8" t="s">
         <v>28</v>
@@ -6466,7 +6466,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="8" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="B155" s="8" t="s">
         <v>6</v>
@@ -6519,7 +6519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A147" sqref="A147:XFD147"/>
     </sheetView>
   </sheetViews>
@@ -6618,7 +6618,7 @@
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>CONCATENATE("UPDATE base_data.glacier_description SET description = '", fr!G16,"' WHERE fk_glacier='",fr!A16,"' AND fk_language_type='fr' AND fk_glacier_description_type ='0'",";")</f>
-        <v>UPDATE base_data.glacier_description SET description = 'Depuis 1914, différents chercheurs ont entrepris des mesures portant sur l''accumulation et la fonte de neige et des névés, ainsi que sur les valeurs de précipitation dans la zone d''accumulation de Claridenfirn. La méthode glaciologique traditionnelle a été appliquée en creusant une fosse à neige jusqu''à la couche d''ocre appliquée l''automne précédent et en mesurant les équivalents en eau. Les soldes annuels spécifiques du bilan de masse ont été déterminés chaque automne depuis 1957 et également régulièrement au printemps sur deux plateaux situés à une altitude comprise entre 2700 et 2900 m.' WHERE fk_glacier='81722f8f-4ec8-11e8-8842-985fd331b2ee' AND fk_language_type='fr' AND fk_glacier_description_type ='0';</v>
+        <v>UPDATE base_data.glacier_description SET description = 'Depuis 1914, différents chercheurs ont entrepris des mesures portant sur l''accumulation et la fonte de neige et des névés, ainsi que sur les valeurs de précipitation dans la zone d''accumulation de Claridenfirn. La méthode glaciologique traditionnelle a été appliquée en creusant une fosse à neige jusqu''à la couche d''ocre appliquée l''automne précédent et en mesurant les équivalents en eau. Les soldes annuels spécifiques du bilan de masse ont été déterminés chaque automne depuis 1957 et également régulièrement au printemps sur deux plateaux situés à une altitude comprise entre 2700 et 2900 m.' WHERE fk_glacier='8176754f-4ec8-11e8-9a29-985fd331b2ee' AND fk_language_type='fr' AND fk_glacier_description_type ='0';</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -6708,7 +6708,7 @@
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>CONCATENATE("UPDATE base_data.glacier_description SET description = '", fr!G31,"' WHERE fk_glacier='",fr!A31,"' AND fk_language_type='fr' AND fk_glacier_description_type ='0'",";")</f>
-        <v>UPDATE base_data.glacier_description SET description = 'Ghiacciaio del Basòdino est un petit glacier de montagne tempéré orienté vers le nord-est dans les Alpes suisses du sud. La petite branche individuelle descendant vers le nord avec une langue distincte n''est pas considérée comme faisant partie du glacier et n''est donc pas incluse dans la détermination du bilan de masse. La branche principale couvre actuellement une superficie de 1.8 km2 et s''étend de 2562 à 3186 m d''altitude. ' WHERE fk_glacier='810ae240-4ec8-11e8-9773-985fd331b2ee' AND fk_language_type='fr' AND fk_glacier_description_type ='0';</v>
+        <v>UPDATE base_data.glacier_description SET description = 'Ghiacciaio del Basòdino est un petit glacier de montagne tempéré orienté vers le nord-est dans les Alpes suisses du sud. La petite branche individuelle descendant vers le nord avec une langue distincte n''est pas considérée comme faisant partie du glacier et n''est donc pas incluse dans la détermination du bilan de masse. La branche principale couvre actuellement une superficie de 1.8 km2 et s''étend de 2562 à 3186 m d''altitude. ' WHERE fk_glacier='81103970-4ec8-11e8-8d3b-985fd331b2ee' AND fk_language_type='fr' AND fk_glacier_description_type ='0';</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -7404,7 +7404,7 @@
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="str">
         <f>CONCATENATE("UPDATE base_data.glacier_description SET description = '", fr!G147,"' WHERE fk_glacier='",fr!A147,"' AND fk_language_type='fr' AND fk_glacier_description_type ='0'",";")</f>
-        <v>UPDATE base_data.glacier_description SET description = 'Le Vadret dal Murtèl est situé dans les Alpes intérieures de Haute-Engadine au sud-est de la Suisse. Le glacier de cirque orienté vers l''est se trouvant près du Piz Corvatsch (3451 m d''altitude) couvre une superficie de 0.3 km2 et reste remarquablement crevassé dans sa partie médiane la plus abrupte. N''exposant que très peu de débris au pied des hautes parois confinant le glacier au nord et à l''ouest, le Vadret dal Murtèl est un glacier typique de glace de surface pure.' WHERE fk_glacier='81e98270-4ec8-11e8-86b3-985fd331b2ee' AND fk_language_type='fr' AND fk_glacier_description_type ='0';</v>
+        <v>UPDATE base_data.glacier_description SET description = 'Le Vadret dal Murtèl est situé dans les Alpes intérieures de Haute-Engadine au sud-est de la Suisse. Le glacier de cirque orienté vers l''est se trouvant près du Piz Corvatsch (3451 m d''altitude) couvre une superficie de 0.3 km2 et reste remarquablement crevassé dans sa partie médiane la plus abrupte. N''exposant que très peu de débris au pied des hautes parois confinant le glacier au nord et à l''ouest, le Vadret dal Murtèl est un glacier typique de glace de surface pure.' WHERE fk_glacier='81ed04e1-4ec8-11e8-a1f7-985fd331b2ee' AND fk_language_type='fr' AND fk_glacier_description_type ='0';</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
@@ -7472,777 +7472,777 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
     </row>
   </sheetData>
@@ -8262,12 +8262,12 @@
   <sheetData>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>